<commit_message>
classes base + backlog
</commit_message>
<xml_diff>
--- a/RockPaperSciccors_BackLog.xlsx
+++ b/RockPaperSciccors_BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wiebe\Documents\Projects\Rock Paper Sciccors - C++ &amp; Qt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09B75756-E318-4159-BB61-B6299842EA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07293D92-29CC-40CB-BD8C-33A57D87728F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{B83C7025-0C3E-4FA9-A572-4D8F53DA8C10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>M2 - Terminal Functionality</t>
   </si>
@@ -538,7 +538,7 @@
   <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -561,6 +561,7 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
@@ -574,81 +575,99 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="2:4" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="2:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>10</v>
       </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>8</v>
       </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>9</v>
       </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" t="s">
         <v>11</v>
       </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:4" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>12</v>
       </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
         <v>15</v>
       </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
         <v>18</v>
       </c>
+      <c r="D21" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:D21">

</xml_diff>